<commit_message>
Various tweaks to Excel importer / exporter and add unit tests
</commit_message>
<xml_diff>
--- a/tests/unittests/excel/data/formula.xlsx
+++ b/tests/unittests/excel/data/formula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\jaqy\tests\unittests\excel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B81A84B9-0765-4FD4-9F77-BAE1B98220FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C567BA-FA35-4398-AA01-3B147ABC0FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{CC7E6383-883E-41A5-82FA-0FAD1FB5513D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Id</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Cos</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Something</t>
   </si>
 </sst>
 </file>
@@ -394,15 +400,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D08475-954F-42DC-8E66-726B19CD6A03}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +421,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -425,8 +440,11 @@
         <f>COS(A2)</f>
         <v>0.54030230586813977</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -439,8 +457,12 @@
         <f t="shared" ref="C3:C16" si="1">COS(A3)</f>
         <v>-0.41614683654714241</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT(D2,"a")</f>
+        <v>1a</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A16" si="2">A3+1</f>
         <v>3</v>
@@ -453,8 +475,12 @@
         <f t="shared" si="1"/>
         <v>-0.98999249660044542</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D16" si="3">_xlfn.CONCAT(D3,"a")</f>
+        <v>1aa</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -467,8 +493,12 @@
         <f t="shared" si="1"/>
         <v>-0.65364362086361194</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaa</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -481,8 +511,12 @@
         <f t="shared" si="1"/>
         <v>0.28366218546322625</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaa</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -495,8 +529,12 @@
         <f t="shared" si="1"/>
         <v>0.96017028665036597</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaa</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -509,8 +547,12 @@
         <f t="shared" si="1"/>
         <v>0.7539022543433046</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaa</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -523,8 +565,12 @@
         <f t="shared" si="1"/>
         <v>-0.14550003380861354</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaa</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -537,8 +583,12 @@
         <f t="shared" si="1"/>
         <v>-0.91113026188467694</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaaa</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -551,8 +601,12 @@
         <f t="shared" si="1"/>
         <v>-0.83907152907645244</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaaaa</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -565,8 +619,12 @@
         <f t="shared" si="1"/>
         <v>4.4256979880507854E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaaaaa</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -579,8 +637,12 @@
         <f t="shared" si="1"/>
         <v>0.84385395873249214</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaaaaaa</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -593,8 +655,12 @@
         <f t="shared" si="1"/>
         <v>0.90744678145019619</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaaaaaaa</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -607,8 +673,12 @@
         <f t="shared" si="1"/>
         <v>0.13673721820783361</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaaaaaaaa</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -620,6 +690,10 @@
       <c r="C16">
         <f t="shared" si="1"/>
         <v>-0.75968791285882131</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="3"/>
+        <v>1aaaaaaaaaaaaaa</v>
       </c>
     </row>
   </sheetData>

</xml_diff>